<commit_message>
added CTVA and LNN
</commit_message>
<xml_diff>
--- a/agtechbioscience_companies.xlsx
+++ b/agtechbioscience_companies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/32906c935fa0eb4f/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="207" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D02B6501-239A-46DB-97B8-96B1744A7021}"/>
+  <xr:revisionPtr revIDLastSave="210" documentId="11_F25DC773A252ABDACC104889191A52245ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F40431B4-7FC8-4B40-812A-474B1673E63F}"/>
   <bookViews>
-    <workbookView xWindow="38780" yWindow="0" windowWidth="17190" windowHeight="15850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1300" yWindow="630" windowWidth="17900" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Private" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="150">
   <si>
     <t>Company Name</t>
   </si>
@@ -504,6 +504,15 @@
   </si>
   <si>
     <t>ALTG</t>
+  </si>
+  <si>
+    <t>AGCO</t>
+  </si>
+  <si>
+    <t>CTVA</t>
+  </si>
+  <si>
+    <t>FAMC</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDF9ECE1-1192-4F7A-A362-8E5BDDDCBEF2}">
   <dimension ref="B2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1072,6 +1081,9 @@
       <c r="B3" t="s">
         <v>34</v>
       </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
       <c r="D3" t="s">
         <v>54</v>
       </c>
@@ -1218,6 +1230,9 @@
       <c r="B16" t="s">
         <v>73</v>
       </c>
+      <c r="C16" t="s">
+        <v>148</v>
+      </c>
       <c r="D16" t="s">
         <v>75</v>
       </c>
@@ -1308,6 +1323,9 @@
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>149</v>
       </c>
       <c r="D24" t="s">
         <v>93</v>

</xml_diff>